<commit_message>
Update PAG and VIL report
</commit_message>
<xml_diff>
--- a/PAG/Report/tables/pag-reliability.xlsx
+++ b/PAG/Report/tables/pag-reliability.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OP18REFCS03\Stations\PAG\Report\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PlantAudit\PAG\Report\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708D707E-4B7B-4572-9E98-CA6263DEB779}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C13C649-693F-4382-9CFE-9646C9366F84}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0B290FBB-465A-489C-89D0-C7FC0DD408BB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0B290FBB-465A-489C-89D0-C7FC0DD408BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Failure Data" sheetId="1" r:id="rId1"/>
@@ -144,7 +144,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -179,7 +179,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -499,13 +499,13 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.08984375" customWidth="1"/>
+    <col min="2" max="2" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.36328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.1796875" bestFit="1" customWidth="1"/>
@@ -588,7 +588,7 @@
         <v>0.18472222222222223</v>
       </c>
       <c r="O2" s="5">
-        <f>(C2-B2)*24</f>
+        <f t="shared" ref="O2:O18" si="0">(C2-B2)*24</f>
         <v>0</v>
       </c>
       <c r="P2" t="s">
@@ -622,7 +622,7 @@
         <v>0.28611111111111109</v>
       </c>
       <c r="O3" s="5">
-        <f>(C3-B3)*24</f>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
     </row>
@@ -637,7 +637,7 @@
         <v>34</v>
       </c>
       <c r="O4" s="5">
-        <f>(C4-B4)*24</f>
+        <f t="shared" si="0"/>
         <v>-1014960</v>
       </c>
     </row>
@@ -674,7 +674,7 @@
         <v>0.27083333333333326</v>
       </c>
       <c r="O5" s="5">
-        <f>(C5-B5)*24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -689,7 +689,7 @@
         <v>34</v>
       </c>
       <c r="O6" s="5">
-        <f>(C6-B6)*24</f>
+        <f t="shared" si="0"/>
         <v>-1014960</v>
       </c>
     </row>
@@ -729,7 +729,7 @@
         <v>0.41666666666666674</v>
       </c>
       <c r="O7" s="5">
-        <f>(C7-B7)*24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -769,7 +769,7 @@
         <v>0.20833333333333331</v>
       </c>
       <c r="O8" s="5">
-        <f>(C8-B8)*24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -809,7 +809,7 @@
         <v>42757.209722222222</v>
       </c>
       <c r="O9" s="5">
-        <f>(C9-B9)*24</f>
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
     </row>
@@ -831,7 +831,7 @@
         <v>-0.91666666666666663</v>
       </c>
       <c r="O10" s="5">
-        <f>(C10-B10)*24</f>
+        <f t="shared" si="0"/>
         <v>-1015200</v>
       </c>
       <c r="P10" t="s">
@@ -849,7 +849,7 @@
         <v>34</v>
       </c>
       <c r="O11" s="5">
-        <f>(C11-B11)*24</f>
+        <f t="shared" si="0"/>
         <v>-1015200</v>
       </c>
       <c r="P11" t="s">
@@ -883,11 +883,11 @@
         <v>0.81597222222222221</v>
       </c>
       <c r="N12" s="3">
-        <f>M12-L12</f>
+        <f t="shared" ref="N12:N18" si="1">M12-L12</f>
         <v>0.55208333333333326</v>
       </c>
       <c r="O12" s="5">
-        <f>(C12-B12)*24</f>
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
     </row>
@@ -914,11 +914,11 @@
         <v>0.48958333333333331</v>
       </c>
       <c r="N13" s="3">
-        <f>M13-L13</f>
+        <f t="shared" si="1"/>
         <v>-0.13541666666666669</v>
       </c>
       <c r="O13" s="5">
-        <f>(C13-B13)*24</f>
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
     </row>
@@ -945,11 +945,11 @@
         <v>0.92013888888888884</v>
       </c>
       <c r="N14" s="3">
-        <f>M14-L14</f>
+        <f t="shared" si="1"/>
         <v>0.12847222222222221</v>
       </c>
       <c r="O14" s="5">
-        <f>(C14-B14)*24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -982,11 +982,11 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="N15" s="3">
-        <f>M15-L15</f>
+        <f t="shared" si="1"/>
         <v>0.16874999999999996</v>
       </c>
       <c r="O15" s="5">
-        <f>(C15-B15)*24</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="P15" t="s">
@@ -1022,11 +1022,11 @@
         <v>0.20833333333333334</v>
       </c>
       <c r="N16" s="3">
-        <f>M16-L16</f>
+        <f t="shared" si="1"/>
         <v>-0.625</v>
       </c>
       <c r="O16" s="5">
-        <f>(C16-B16)*24</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
@@ -1056,11 +1056,11 @@
         <v>0.14930555555555555</v>
       </c>
       <c r="N17" s="3">
-        <f>M17-L17</f>
+        <f t="shared" si="1"/>
         <v>-0.72569444444444442</v>
       </c>
       <c r="O17" s="5">
-        <f>(C17-B17)*24</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
@@ -1093,11 +1093,11 @@
         <v>0.69374999999999998</v>
       </c>
       <c r="N18" s="3">
-        <f>M18-L18</f>
+        <f t="shared" si="1"/>
         <v>0.17291666666666661</v>
       </c>
       <c r="O18" s="5">
-        <f>(C18-B18)*24</f>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="Q18" t="s">

</xml_diff>